<commit_message>
WDZO-1321: changed templates for uploading/deleting users
</commit_message>
<xml_diff>
--- a/public/templates/user-upload.xlsx
+++ b/public/templates/user-upload.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dk/IdeaProjects/distributor-admin/public/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u18591523/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C74B1E63-E982-EC41-AB57-7E9713C6DFDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C161D5-2A90-494D-B869-CA70A439543B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Табельный номер сотрудника</t>
   </si>
@@ -46,71 +46,44 @@
     <t>Александрович</t>
   </si>
   <si>
-    <t>428_8588_51113</t>
-  </si>
-  <si>
     <t>37887638</t>
   </si>
   <si>
-    <t>603_5256_67179</t>
-  </si>
-  <si>
     <t>48978837</t>
   </si>
   <si>
-    <t>297_8539_86279</t>
-  </si>
-  <si>
-    <t>17201721</t>
-  </si>
-  <si>
-    <t>681_4747_71856</t>
-  </si>
-  <si>
-    <t>87929738</t>
-  </si>
-  <si>
-    <t>165_2936_53097</t>
-  </si>
-  <si>
-    <t>24068385</t>
-  </si>
-  <si>
-    <t>313_3317_95009</t>
-  </si>
-  <si>
-    <t>93936960</t>
-  </si>
-  <si>
-    <t>264_9236_57239</t>
-  </si>
-  <si>
-    <t>91563671</t>
-  </si>
-  <si>
-    <t>718_3387_77812</t>
-  </si>
-  <si>
-    <t>27243099</t>
-  </si>
-  <si>
-    <t>522_9443_48594</t>
-  </si>
-  <si>
-    <t>36144935</t>
-  </si>
-  <si>
-    <t>360_1673_68217</t>
-  </si>
-  <si>
     <t>Точка продажи</t>
+  </si>
+  <si>
+    <t>Екатерина</t>
+  </si>
+  <si>
+    <t>Федоровна</t>
+  </si>
+  <si>
+    <t>д’Артаньян</t>
+  </si>
+  <si>
+    <t>Плотникова-Работникова</t>
+  </si>
+  <si>
+    <t>Артем</t>
+  </si>
+  <si>
+    <t>Петрович</t>
+  </si>
+  <si>
+    <t>038_9038_0393</t>
+  </si>
+  <si>
+    <t>Удали содержимое и используй как шаблон ツ</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -122,10 +95,23 @@
       <b/>
       <sz val="12.5"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12.5"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.5"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12.5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -159,10 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -479,7 +467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -500,7 +490,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -517,161 +507,93 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>20</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
-      </c>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>